<commit_message>
Ajout de graphe et prise en compte de l'elo estimé
</commit_message>
<xml_diff>
--- a/chessResultsList.xlsx
+++ b/chessResultsList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\Python\Seminaire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002486F2-0118-4197-8135-A7FF0DC75B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9550CF-425F-42E1-98FE-3260717AC4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="1183">
   <si>
     <t>Rk.</t>
   </si>
@@ -3161,6 +3161,414 @@
   </si>
   <si>
     <t>268b1</t>
+  </si>
+  <si>
+    <t>Rp</t>
+  </si>
+  <si>
+    <t>3408</t>
+  </si>
+  <si>
+    <t>2796</t>
+  </si>
+  <si>
+    <t>2745</t>
+  </si>
+  <si>
+    <t>2710</t>
+  </si>
+  <si>
+    <t>2781</t>
+  </si>
+  <si>
+    <t>2794</t>
+  </si>
+  <si>
+    <t>2736</t>
+  </si>
+  <si>
+    <t>2784</t>
+  </si>
+  <si>
+    <t>2702</t>
+  </si>
+  <si>
+    <t>2762</t>
+  </si>
+  <si>
+    <t>2750</t>
+  </si>
+  <si>
+    <t>2696</t>
+  </si>
+  <si>
+    <t>2728</t>
+  </si>
+  <si>
+    <t>2669</t>
+  </si>
+  <si>
+    <t>2714</t>
+  </si>
+  <si>
+    <t>2719</t>
+  </si>
+  <si>
+    <t>2678</t>
+  </si>
+  <si>
+    <t>2639</t>
+  </si>
+  <si>
+    <t>2646</t>
+  </si>
+  <si>
+    <t>2629</t>
+  </si>
+  <si>
+    <t>2585</t>
+  </si>
+  <si>
+    <t>2620</t>
+  </si>
+  <si>
+    <t>2627</t>
+  </si>
+  <si>
+    <t>2596</t>
+  </si>
+  <si>
+    <t>2668</t>
+  </si>
+  <si>
+    <t>2621</t>
+  </si>
+  <si>
+    <t>2683</t>
+  </si>
+  <si>
+    <t>2587</t>
+  </si>
+  <si>
+    <t>2605</t>
+  </si>
+  <si>
+    <t>2630</t>
+  </si>
+  <si>
+    <t>2584</t>
+  </si>
+  <si>
+    <t>2644</t>
+  </si>
+  <si>
+    <t>2659</t>
+  </si>
+  <si>
+    <t>2562</t>
+  </si>
+  <si>
+    <t>2649</t>
+  </si>
+  <si>
+    <t>2640</t>
+  </si>
+  <si>
+    <t>2570</t>
+  </si>
+  <si>
+    <t>2684</t>
+  </si>
+  <si>
+    <t>2634</t>
+  </si>
+  <si>
+    <t>2554</t>
+  </si>
+  <si>
+    <t>2588</t>
+  </si>
+  <si>
+    <t>2626</t>
+  </si>
+  <si>
+    <t>2603</t>
+  </si>
+  <si>
+    <t>2573</t>
+  </si>
+  <si>
+    <t>2552</t>
+  </si>
+  <si>
+    <t>2512</t>
+  </si>
+  <si>
+    <t>2543</t>
+  </si>
+  <si>
+    <t>2499</t>
+  </si>
+  <si>
+    <t>2532</t>
+  </si>
+  <si>
+    <t>2401</t>
+  </si>
+  <si>
+    <t>2575</t>
+  </si>
+  <si>
+    <t>2564</t>
+  </si>
+  <si>
+    <t>2504</t>
+  </si>
+  <si>
+    <t>2559</t>
+  </si>
+  <si>
+    <t>2526</t>
+  </si>
+  <si>
+    <t>2523</t>
+  </si>
+  <si>
+    <t>2467</t>
+  </si>
+  <si>
+    <t>2410</t>
+  </si>
+  <si>
+    <t>2524</t>
+  </si>
+  <si>
+    <t>2471</t>
+  </si>
+  <si>
+    <t>2453</t>
+  </si>
+  <si>
+    <t>2424</t>
+  </si>
+  <si>
+    <t>2426</t>
+  </si>
+  <si>
+    <t>2409</t>
+  </si>
+  <si>
+    <t>2509</t>
+  </si>
+  <si>
+    <t>2364</t>
+  </si>
+  <si>
+    <t>2407</t>
+  </si>
+  <si>
+    <t>2352</t>
+  </si>
+  <si>
+    <t>2357</t>
+  </si>
+  <si>
+    <t>2278</t>
+  </si>
+  <si>
+    <t>2263</t>
+  </si>
+  <si>
+    <t>2284</t>
+  </si>
+  <si>
+    <t>2253</t>
+  </si>
+  <si>
+    <t>2304</t>
+  </si>
+  <si>
+    <t>2494</t>
+  </si>
+  <si>
+    <t>2540</t>
+  </si>
+  <si>
+    <t>2415</t>
+  </si>
+  <si>
+    <t>2439</t>
+  </si>
+  <si>
+    <t>2396</t>
+  </si>
+  <si>
+    <t>2338</t>
+  </si>
+  <si>
+    <t>2240</t>
+  </si>
+  <si>
+    <t>2427</t>
+  </si>
+  <si>
+    <t>2411</t>
+  </si>
+  <si>
+    <t>2405</t>
+  </si>
+  <si>
+    <t>2314</t>
+  </si>
+  <si>
+    <t>2398</t>
+  </si>
+  <si>
+    <t>2406</t>
+  </si>
+  <si>
+    <t>2311</t>
+  </si>
+  <si>
+    <t>2319</t>
+  </si>
+  <si>
+    <t>2336</t>
+  </si>
+  <si>
+    <t>2380</t>
+  </si>
+  <si>
+    <t>2257</t>
+  </si>
+  <si>
+    <t>2239</t>
+  </si>
+  <si>
+    <t>2330</t>
+  </si>
+  <si>
+    <t>2610</t>
+  </si>
+  <si>
+    <t>2309</t>
+  </si>
+  <si>
+    <t>2316</t>
+  </si>
+  <si>
+    <t>2167</t>
+  </si>
+  <si>
+    <t>2344</t>
+  </si>
+  <si>
+    <t>2251</t>
+  </si>
+  <si>
+    <t>2234</t>
+  </si>
+  <si>
+    <t>2312</t>
+  </si>
+  <si>
+    <t>2276</t>
+  </si>
+  <si>
+    <t>2190</t>
+  </si>
+  <si>
+    <t>2203</t>
+  </si>
+  <si>
+    <t>2296</t>
+  </si>
+  <si>
+    <t>2341</t>
+  </si>
+  <si>
+    <t>2391</t>
+  </si>
+  <si>
+    <t>2237</t>
+  </si>
+  <si>
+    <t>2358</t>
+  </si>
+  <si>
+    <t>2399</t>
+  </si>
+  <si>
+    <t>2242</t>
+  </si>
+  <si>
+    <t>2259</t>
+  </si>
+  <si>
+    <t>2249</t>
+  </si>
+  <si>
+    <t>2288</t>
+  </si>
+  <si>
+    <t>2294</t>
+  </si>
+  <si>
+    <t>2390</t>
+  </si>
+  <si>
+    <t>2261</t>
+  </si>
+  <si>
+    <t>2207</t>
+  </si>
+  <si>
+    <t>2243</t>
+  </si>
+  <si>
+    <t>2258</t>
+  </si>
+  <si>
+    <t>2221</t>
+  </si>
+  <si>
+    <t>2228</t>
+  </si>
+  <si>
+    <t>2185</t>
+  </si>
+  <si>
+    <t>2348</t>
+  </si>
+  <si>
+    <t>2282</t>
+  </si>
+  <si>
+    <t>2181</t>
+  </si>
+  <si>
+    <t>2292</t>
+  </si>
+  <si>
+    <t>2209</t>
+  </si>
+  <si>
+    <t>2270</t>
+  </si>
+  <si>
+    <t>2123</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>2107</t>
+  </si>
+  <si>
+    <t>2136</t>
+  </si>
+  <si>
+    <t>2191</t>
   </si>
 </sst>
 </file>
@@ -3248,7 +3656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3267,6 +3675,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10327,10 +10741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q154"/>
+  <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="U150" sqref="U150"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10345,7 +10759,7 @@
     <col min="17" max="17" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -10393,8 +10807,11 @@
       <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="R1" s="10" t="s">
+        <v>1047</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -10446,8 +10863,11 @@
       <c r="Q2" s="4">
         <v>52.5</v>
       </c>
+      <c r="R2" s="9" t="s">
+        <v>1048</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -10499,8 +10919,11 @@
       <c r="Q3" s="4">
         <v>52.5</v>
       </c>
+      <c r="R3" s="9" t="s">
+        <v>1049</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -10552,8 +10975,11 @@
       <c r="Q4" s="4">
         <v>52</v>
       </c>
+      <c r="R4" s="9" t="s">
+        <v>1050</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
@@ -10603,8 +11029,11 @@
       <c r="Q5" s="4">
         <v>52</v>
       </c>
+      <c r="R5" s="9" t="s">
+        <v>1051</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -10656,8 +11085,11 @@
       <c r="Q6" s="4">
         <v>50.5</v>
       </c>
+      <c r="R6" s="9" t="s">
+        <v>1052</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="3" t="s">
         <v>15</v>
@@ -10707,8 +11139,11 @@
       <c r="Q7" s="4">
         <v>50.5</v>
       </c>
+      <c r="R7" s="9" t="s">
+        <v>1053</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -10760,8 +11195,11 @@
       <c r="Q8" s="4">
         <v>50</v>
       </c>
+      <c r="R8" s="9" t="s">
+        <v>1054</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -10811,8 +11249,11 @@
       <c r="Q9" s="4">
         <v>50</v>
       </c>
+      <c r="R9" s="9" t="s">
+        <v>1055</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -10864,8 +11305,11 @@
       <c r="Q10" s="4">
         <v>56</v>
       </c>
+      <c r="R10" s="9" t="s">
+        <v>1056</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -10917,8 +11361,11 @@
       <c r="Q11" s="4">
         <v>54</v>
       </c>
+      <c r="R11" s="9" t="s">
+        <v>1057</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -10970,8 +11417,11 @@
       <c r="Q12" s="4">
         <v>53</v>
       </c>
+      <c r="R12" s="9" t="s">
+        <v>1058</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -11023,8 +11473,11 @@
       <c r="Q13" s="4">
         <v>52.5</v>
       </c>
+      <c r="R13" s="9" t="s">
+        <v>1059</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -11076,8 +11529,11 @@
       <c r="Q14" s="4">
         <v>52</v>
       </c>
+      <c r="R14" s="9" t="s">
+        <v>1060</v>
+      </c>
     </row>
-    <row r="15" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -11129,8 +11585,11 @@
       <c r="Q15" s="4">
         <v>50.5</v>
       </c>
+      <c r="R15" s="9" t="s">
+        <v>1061</v>
+      </c>
     </row>
-    <row r="16" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
         <v>15</v>
@@ -11180,8 +11639,11 @@
       <c r="Q16" s="4">
         <v>50.5</v>
       </c>
+      <c r="R16" s="9" t="s">
+        <v>1062</v>
+      </c>
     </row>
-    <row r="17" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -11233,8 +11695,11 @@
       <c r="Q17" s="4">
         <v>50</v>
       </c>
+      <c r="R17" s="9" t="s">
+        <v>1063</v>
+      </c>
     </row>
-    <row r="18" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
         <v>15</v>
@@ -11284,8 +11749,11 @@
       <c r="Q18" s="4">
         <v>50</v>
       </c>
+      <c r="R18" s="9" t="s">
+        <v>1064</v>
+      </c>
     </row>
-    <row r="19" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -11337,8 +11805,11 @@
       <c r="Q19" s="4">
         <v>49.5</v>
       </c>
+      <c r="R19" s="9" t="s">
+        <v>1062</v>
+      </c>
     </row>
-    <row r="20" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -11390,8 +11861,11 @@
       <c r="Q20" s="4">
         <v>49</v>
       </c>
+      <c r="R20" s="9" t="s">
+        <v>1065</v>
+      </c>
     </row>
-    <row r="21" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
         <v>15</v>
@@ -11441,8 +11915,11 @@
       <c r="Q21" s="4">
         <v>49</v>
       </c>
+      <c r="R21" s="9" t="s">
+        <v>1066</v>
+      </c>
     </row>
-    <row r="22" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
         <v>15</v>
@@ -11492,8 +11969,11 @@
       <c r="Q22" s="4">
         <v>49</v>
       </c>
+      <c r="R22" s="9" t="s">
+        <v>1067</v>
+      </c>
     </row>
-    <row r="23" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -11545,8 +12025,11 @@
       <c r="Q23" s="4">
         <v>48.5</v>
       </c>
+      <c r="R23" s="9" t="s">
+        <v>1068</v>
+      </c>
     </row>
-    <row r="24" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -11598,8 +12081,11 @@
       <c r="Q24" s="4">
         <v>48</v>
       </c>
+      <c r="R24" s="9" t="s">
+        <v>1069</v>
+      </c>
     </row>
-    <row r="25" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -11651,8 +12137,11 @@
       <c r="Q25" s="4">
         <v>47.5</v>
       </c>
+      <c r="R25" s="9" t="s">
+        <v>1070</v>
+      </c>
     </row>
-    <row r="26" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -11704,8 +12193,11 @@
       <c r="Q26" s="4">
         <v>55.5</v>
       </c>
+      <c r="R26" s="9" t="s">
+        <v>1071</v>
+      </c>
     </row>
-    <row r="27" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -11757,8 +12249,11 @@
       <c r="Q27" s="4">
         <v>54</v>
       </c>
+      <c r="R27" s="9" t="s">
+        <v>1072</v>
+      </c>
     </row>
-    <row r="28" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -11810,8 +12305,11 @@
       <c r="Q28" s="4">
         <v>53.5</v>
       </c>
+      <c r="R28" s="9" t="s">
+        <v>1073</v>
+      </c>
     </row>
-    <row r="29" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="3" t="s">
         <v>15</v>
@@ -11861,8 +12359,11 @@
       <c r="Q29" s="4">
         <v>53.5</v>
       </c>
+      <c r="R29" s="9" t="s">
+        <v>1074</v>
+      </c>
     </row>
-    <row r="30" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -11914,8 +12415,11 @@
       <c r="Q30" s="4">
         <v>52.5</v>
       </c>
+      <c r="R30" s="9" t="s">
+        <v>1075</v>
+      </c>
     </row>
-    <row r="31" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -11967,8 +12471,11 @@
       <c r="Q31" s="4">
         <v>51.5</v>
       </c>
+      <c r="R31" s="9" t="s">
+        <v>1076</v>
+      </c>
     </row>
-    <row r="32" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="3" t="s">
         <v>15</v>
@@ -12018,8 +12525,11 @@
       <c r="Q32" s="4">
         <v>51.5</v>
       </c>
+      <c r="R32" s="9" t="s">
+        <v>1077</v>
+      </c>
     </row>
-    <row r="33" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -12071,8 +12581,11 @@
       <c r="Q33" s="4">
         <v>51</v>
       </c>
+      <c r="R33" s="9" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="34" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -12124,8 +12637,11 @@
       <c r="Q34" s="4">
         <v>50.5</v>
       </c>
+      <c r="R34" s="9" t="s">
+        <v>1079</v>
+      </c>
     </row>
-    <row r="35" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="3" t="s">
         <v>15</v>
@@ -12175,8 +12691,11 @@
       <c r="Q35" s="4">
         <v>50.5</v>
       </c>
+      <c r="R35" s="9" t="s">
+        <v>1080</v>
+      </c>
     </row>
-    <row r="36" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="3" t="s">
         <v>15</v>
@@ -12226,8 +12745,11 @@
       <c r="Q36" s="4">
         <v>50.5</v>
       </c>
+      <c r="R36" s="9" t="s">
+        <v>1081</v>
+      </c>
     </row>
-    <row r="37" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -12279,8 +12801,11 @@
       <c r="Q37" s="4">
         <v>50</v>
       </c>
+      <c r="R37" s="9" t="s">
+        <v>1082</v>
+      </c>
     </row>
-    <row r="38" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="3" t="s">
         <v>15</v>
@@ -12330,8 +12855,11 @@
       <c r="Q38" s="4">
         <v>50</v>
       </c>
+      <c r="R38" s="9" t="s">
+        <v>1083</v>
+      </c>
     </row>
-    <row r="39" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="3" t="s">
         <v>15</v>
@@ -12381,8 +12909,11 @@
       <c r="Q39" s="4">
         <v>50</v>
       </c>
+      <c r="R39" s="9" t="s">
+        <v>1084</v>
+      </c>
     </row>
-    <row r="40" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -12434,8 +12965,11 @@
       <c r="Q40" s="4">
         <v>49.5</v>
       </c>
+      <c r="R40" s="9" t="s">
+        <v>1070</v>
+      </c>
     </row>
-    <row r="41" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="3" t="s">
         <v>15</v>
@@ -12485,8 +13019,11 @@
       <c r="Q41" s="4">
         <v>49.5</v>
       </c>
+      <c r="R41" s="9" t="s">
+        <v>1085</v>
+      </c>
     </row>
-    <row r="42" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="3" t="s">
         <v>15</v>
@@ -12536,8 +13073,11 @@
       <c r="Q42" s="4">
         <v>49.5</v>
       </c>
+      <c r="R42" s="9" t="s">
+        <v>1086</v>
+      </c>
     </row>
-    <row r="43" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -12589,8 +13129,11 @@
       <c r="Q43" s="4">
         <v>49</v>
       </c>
+      <c r="R43" s="9" t="s">
+        <v>1087</v>
+      </c>
     </row>
-    <row r="44" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="3" t="s">
         <v>15</v>
@@ -12640,8 +13183,11 @@
       <c r="Q44" s="4">
         <v>49</v>
       </c>
+      <c r="R44" s="9" t="s">
+        <v>1088</v>
+      </c>
     </row>
-    <row r="45" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -12693,8 +13239,11 @@
       <c r="Q45" s="4">
         <v>48.5</v>
       </c>
+      <c r="R45" s="9" t="s">
+        <v>1089</v>
+      </c>
     </row>
-    <row r="46" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -12746,8 +13295,11 @@
       <c r="Q46" s="4">
         <v>48</v>
       </c>
+      <c r="R46" s="9" t="s">
+        <v>1090</v>
+      </c>
     </row>
-    <row r="47" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -12799,8 +13351,11 @@
       <c r="Q47" s="4">
         <v>47.5</v>
       </c>
+      <c r="R47" s="9" t="s">
+        <v>1091</v>
+      </c>
     </row>
-    <row r="48" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="3" t="s">
         <v>15</v>
@@ -12850,8 +13405,11 @@
       <c r="Q48" s="4">
         <v>47.5</v>
       </c>
+      <c r="R48" s="9" t="s">
+        <v>1088</v>
+      </c>
     </row>
-    <row r="49" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="3" t="s">
         <v>15</v>
@@ -12901,8 +13459,11 @@
       <c r="Q49" s="4">
         <v>47.5</v>
       </c>
+      <c r="R49" s="9" t="s">
+        <v>1075</v>
+      </c>
     </row>
-    <row r="50" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4"/>
       <c r="B50" s="3" t="s">
         <v>15</v>
@@ -12952,8 +13513,11 @@
       <c r="Q50" s="4">
         <v>47.5</v>
       </c>
+      <c r="R50" s="9" t="s">
+        <v>1092</v>
+      </c>
     </row>
-    <row r="51" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4"/>
       <c r="B51" s="3" t="s">
         <v>15</v>
@@ -13003,8 +13567,11 @@
       <c r="Q51" s="4">
         <v>47.5</v>
       </c>
+      <c r="R51" s="9" t="s">
+        <v>1093</v>
+      </c>
     </row>
-    <row r="52" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -13056,8 +13623,11 @@
       <c r="Q52" s="4">
         <v>47</v>
       </c>
+      <c r="R52" s="9" t="s">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="53" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -13109,8 +13679,11 @@
       <c r="Q53" s="4">
         <v>45</v>
       </c>
+      <c r="R53" s="9" t="s">
+        <v>1095</v>
+      </c>
     </row>
-    <row r="54" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -13162,8 +13735,11 @@
       <c r="Q54" s="4">
         <v>42.5</v>
       </c>
+      <c r="R54" s="9" t="s">
+        <v>1096</v>
+      </c>
     </row>
-    <row r="55" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -13215,8 +13791,11 @@
       <c r="Q55" s="4">
         <v>38.5</v>
       </c>
+      <c r="R55" s="9" t="s">
+        <v>1097</v>
+      </c>
     </row>
-    <row r="56" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -13268,8 +13847,11 @@
       <c r="Q56" s="4">
         <v>50</v>
       </c>
+      <c r="R56" s="9" t="s">
+        <v>1098</v>
+      </c>
     </row>
-    <row r="57" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -13321,8 +13903,11 @@
       <c r="Q57" s="4">
         <v>49.5</v>
       </c>
+      <c r="R57" s="9" t="s">
+        <v>1099</v>
+      </c>
     </row>
-    <row r="58" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="3" t="s">
         <v>15</v>
@@ -13372,8 +13957,11 @@
       <c r="Q58" s="4">
         <v>49.5</v>
       </c>
+      <c r="R58" s="9" t="s">
+        <v>1100</v>
+      </c>
     </row>
-    <row r="59" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -13425,8 +14013,11 @@
       <c r="Q59" s="4">
         <v>49</v>
       </c>
+      <c r="R59" s="9" t="s">
+        <v>1101</v>
+      </c>
     </row>
-    <row r="60" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -13478,8 +14069,11 @@
       <c r="Q60" s="4">
         <v>48</v>
       </c>
+      <c r="R60" s="9" t="s">
+        <v>1102</v>
+      </c>
     </row>
-    <row r="61" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="3" t="s">
         <v>15</v>
@@ -13529,8 +14123,11 @@
       <c r="Q61" s="4">
         <v>48</v>
       </c>
+      <c r="R61" s="9" t="s">
+        <v>1103</v>
+      </c>
     </row>
-    <row r="62" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -13582,8 +14179,11 @@
       <c r="Q62" s="4">
         <v>47.5</v>
       </c>
+      <c r="R62" s="9" t="s">
+        <v>1104</v>
+      </c>
     </row>
-    <row r="63" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="3" t="s">
         <v>15</v>
@@ -13633,8 +14233,11 @@
       <c r="Q63" s="4">
         <v>47.5</v>
       </c>
+      <c r="R63" s="9" t="s">
+        <v>1105</v>
+      </c>
     </row>
-    <row r="64" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -13686,8 +14289,11 @@
       <c r="Q64" s="4">
         <v>46.5</v>
       </c>
+      <c r="R64" s="9" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="65" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -13737,8 +14343,11 @@
       <c r="Q65" s="4">
         <v>46</v>
       </c>
+      <c r="R65" s="9" t="s">
+        <v>1107</v>
+      </c>
     </row>
-    <row r="66" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -13790,8 +14399,11 @@
       <c r="Q66" s="4">
         <v>45</v>
       </c>
+      <c r="R66" s="9" t="s">
+        <v>1108</v>
+      </c>
     </row>
-    <row r="67" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -13843,8 +14455,11 @@
       <c r="Q67" s="4">
         <v>44.5</v>
       </c>
+      <c r="R67" s="9" t="s">
+        <v>1109</v>
+      </c>
     </row>
-    <row r="68" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -13896,8 +14511,11 @@
       <c r="Q68" s="4">
         <v>44</v>
       </c>
+      <c r="R68" s="9" t="s">
+        <v>1110</v>
+      </c>
     </row>
-    <row r="69" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -13949,8 +14567,11 @@
       <c r="Q69" s="4">
         <v>43.5</v>
       </c>
+      <c r="R69" s="9" t="s">
+        <v>1111</v>
+      </c>
     </row>
-    <row r="70" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="3" t="s">
         <v>15</v>
@@ -14000,8 +14621,11 @@
       <c r="Q70" s="4">
         <v>43.5</v>
       </c>
+      <c r="R70" s="9" t="s">
+        <v>1112</v>
+      </c>
     </row>
-    <row r="71" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="3" t="s">
         <v>15</v>
@@ -14051,8 +14675,11 @@
       <c r="Q71" s="4">
         <v>43.5</v>
       </c>
+      <c r="R71" s="9" t="s">
+        <v>1113</v>
+      </c>
     </row>
-    <row r="72" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -14104,8 +14731,11 @@
       <c r="Q72" s="4">
         <v>42.5</v>
       </c>
+      <c r="R72" s="9" t="s">
+        <v>1114</v>
+      </c>
     </row>
-    <row r="73" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -14157,8 +14787,11 @@
       <c r="Q73" s="4">
         <v>41.5</v>
       </c>
+      <c r="R73" s="9" t="s">
+        <v>1115</v>
+      </c>
     </row>
-    <row r="74" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="3" t="s">
         <v>15</v>
@@ -14208,8 +14841,11 @@
       <c r="Q74" s="4">
         <v>41.5</v>
       </c>
+      <c r="R74" s="9" t="s">
+        <v>1116</v>
+      </c>
     </row>
-    <row r="75" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -14261,8 +14897,11 @@
       <c r="Q75" s="4">
         <v>41</v>
       </c>
+      <c r="R75" s="9" t="s">
+        <v>1117</v>
+      </c>
     </row>
-    <row r="76" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="3" t="s">
         <v>15</v>
@@ -14312,8 +14951,11 @@
       <c r="Q76" s="4">
         <v>41</v>
       </c>
+      <c r="R76" s="9" t="s">
+        <v>1105</v>
+      </c>
     </row>
-    <row r="77" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -14365,8 +15007,11 @@
       <c r="Q77" s="4">
         <v>40.5</v>
       </c>
+      <c r="R77" s="9" t="s">
+        <v>1118</v>
+      </c>
     </row>
-    <row r="78" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="3" t="s">
         <v>15</v>
@@ -14416,8 +15061,11 @@
       <c r="Q78" s="4">
         <v>40.5</v>
       </c>
+      <c r="R78" s="9" t="s">
+        <v>1119</v>
+      </c>
     </row>
-    <row r="79" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -14469,8 +15117,11 @@
       <c r="Q79" s="4">
         <v>39.5</v>
       </c>
+      <c r="R79" s="9" t="s">
+        <v>1120</v>
+      </c>
     </row>
-    <row r="80" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -14522,8 +15173,11 @@
       <c r="Q80" s="4">
         <v>37.5</v>
       </c>
+      <c r="R80" s="9" t="s">
+        <v>1121</v>
+      </c>
     </row>
-    <row r="81" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -14575,8 +15229,11 @@
       <c r="Q81" s="4">
         <v>52.5</v>
       </c>
+      <c r="R81" s="9" t="s">
+        <v>1091</v>
+      </c>
     </row>
-    <row r="82" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -14628,8 +15285,11 @@
       <c r="Q82" s="4">
         <v>49.5</v>
       </c>
+      <c r="R82" s="9" t="s">
+        <v>1122</v>
+      </c>
     </row>
-    <row r="83" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -14681,8 +15341,11 @@
       <c r="Q83" s="4">
         <v>48</v>
       </c>
+      <c r="R83" s="9" t="s">
+        <v>1123</v>
+      </c>
     </row>
-    <row r="84" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="3" t="s">
         <v>15</v>
@@ -14730,8 +15393,11 @@
       <c r="Q84" s="4">
         <v>48</v>
       </c>
+      <c r="R84" s="9" t="s">
+        <v>1124</v>
+      </c>
     </row>
-    <row r="85" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -14783,8 +15449,11 @@
       <c r="Q85" s="4">
         <v>47.5</v>
       </c>
+      <c r="R85" s="9" t="s">
+        <v>1125</v>
+      </c>
     </row>
-    <row r="86" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -14836,8 +15505,11 @@
       <c r="Q86" s="4">
         <v>47</v>
       </c>
+      <c r="R86" s="9" t="s">
+        <v>1126</v>
+      </c>
     </row>
-    <row r="87" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -14889,8 +15561,11 @@
       <c r="Q87" s="4">
         <v>44.5</v>
       </c>
+      <c r="R87" s="9" t="s">
+        <v>1127</v>
+      </c>
     </row>
-    <row r="88" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="B88" s="3" t="s">
         <v>15</v>
@@ -14940,8 +15615,11 @@
       <c r="Q88" s="4">
         <v>44.5</v>
       </c>
+      <c r="R88" s="9" t="s">
+        <v>1128</v>
+      </c>
     </row>
-    <row r="89" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4"/>
       <c r="B89" s="3" t="s">
         <v>15</v>
@@ -14991,8 +15669,11 @@
       <c r="Q89" s="4">
         <v>44.5</v>
       </c>
+      <c r="R89" s="9" t="s">
+        <v>1129</v>
+      </c>
     </row>
-    <row r="90" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -15044,8 +15725,11 @@
       <c r="Q90" s="4">
         <v>44</v>
       </c>
+      <c r="R90" s="9" t="s">
+        <v>1130</v>
+      </c>
     </row>
-    <row r="91" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4"/>
       <c r="B91" s="3" t="s">
         <v>15</v>
@@ -15095,8 +15779,11 @@
       <c r="Q91" s="4">
         <v>44</v>
       </c>
+      <c r="R91" s="9" t="s">
+        <v>1131</v>
+      </c>
     </row>
-    <row r="92" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="3" t="s">
         <v>15</v>
@@ -15144,8 +15831,11 @@
       <c r="Q92" s="4">
         <v>44</v>
       </c>
+      <c r="R92" s="9" t="s">
+        <v>1132</v>
+      </c>
     </row>
-    <row r="93" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -15197,8 +15887,11 @@
       <c r="Q93" s="4">
         <v>43.5</v>
       </c>
+      <c r="R93" s="9" t="s">
+        <v>1133</v>
+      </c>
     </row>
-    <row r="94" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="3" t="s">
         <v>15</v>
@@ -15246,8 +15939,11 @@
       <c r="Q94" s="4">
         <v>43.5</v>
       </c>
+      <c r="R94" s="9" t="s">
+        <v>1134</v>
+      </c>
     </row>
-    <row r="95" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -15299,8 +15995,11 @@
       <c r="Q95" s="4">
         <v>43</v>
       </c>
+      <c r="R95" s="9" t="s">
+        <v>1135</v>
+      </c>
     </row>
-    <row r="96" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -15352,8 +16051,11 @@
       <c r="Q96" s="4">
         <v>42.5</v>
       </c>
+      <c r="R96" s="9" t="s">
+        <v>1136</v>
+      </c>
     </row>
-    <row r="97" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -15403,8 +16105,11 @@
       <c r="Q97" s="4">
         <v>41.5</v>
       </c>
+      <c r="R97" s="9" t="s">
+        <v>1137</v>
+      </c>
     </row>
-    <row r="98" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -15454,8 +16159,11 @@
       <c r="Q98" s="4">
         <v>41</v>
       </c>
+      <c r="R98" s="9" t="s">
+        <v>1138</v>
+      </c>
     </row>
-    <row r="99" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -15507,8 +16215,11 @@
       <c r="Q99" s="4">
         <v>40.5</v>
       </c>
+      <c r="R99" s="9" t="s">
+        <v>1139</v>
+      </c>
     </row>
-    <row r="100" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4"/>
       <c r="B100" s="3" t="s">
         <v>15</v>
@@ -15558,8 +16269,11 @@
       <c r="Q100" s="4">
         <v>40.5</v>
       </c>
+      <c r="R100" s="9" t="s">
+        <v>1140</v>
+      </c>
     </row>
-    <row r="101" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4"/>
       <c r="B101" s="3" t="s">
         <v>15</v>
@@ -15607,8 +16321,11 @@
       <c r="Q101" s="4">
         <v>40.5</v>
       </c>
+      <c r="R101" s="9" t="s">
+        <v>1141</v>
+      </c>
     </row>
-    <row r="102" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -15660,8 +16377,11 @@
       <c r="Q102" s="4">
         <v>40</v>
       </c>
+      <c r="R102" s="9" t="s">
+        <v>1142</v>
+      </c>
     </row>
-    <row r="103" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4"/>
       <c r="B103" s="3" t="s">
         <v>15</v>
@@ -15709,8 +16429,11 @@
       <c r="Q103" s="4">
         <v>40</v>
       </c>
+      <c r="R103" s="9" t="s">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="104" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -15762,8 +16485,11 @@
       <c r="Q104" s="4">
         <v>39.5</v>
       </c>
+      <c r="R104" s="9" t="s">
+        <v>1144</v>
+      </c>
     </row>
-    <row r="105" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4"/>
       <c r="B105" s="3" t="s">
         <v>15</v>
@@ -15813,8 +16539,11 @@
       <c r="Q105" s="4">
         <v>39.5</v>
       </c>
+      <c r="R105" s="9" t="s">
+        <v>1145</v>
+      </c>
     </row>
-    <row r="106" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4"/>
       <c r="B106" s="3" t="s">
         <v>15</v>
@@ -15864,8 +16593,11 @@
       <c r="Q106" s="4">
         <v>39.5</v>
       </c>
+      <c r="R106" s="9" t="s">
+        <v>1119</v>
+      </c>
     </row>
-    <row r="107" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4"/>
       <c r="B107" s="3" t="s">
         <v>15</v>
@@ -15913,8 +16645,11 @@
       <c r="Q107" s="4">
         <v>39.5</v>
       </c>
+      <c r="R107" s="9" t="s">
+        <v>1146</v>
+      </c>
     </row>
-    <row r="108" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -15966,8 +16701,11 @@
       <c r="Q108" s="4">
         <v>39</v>
       </c>
+      <c r="R108" s="9" t="s">
+        <v>1147</v>
+      </c>
     </row>
-    <row r="109" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4"/>
       <c r="B109" s="3" t="s">
         <v>15</v>
@@ -16015,8 +16753,11 @@
       <c r="Q109" s="4">
         <v>39</v>
       </c>
+      <c r="R109" s="9" t="s">
+        <v>1148</v>
+      </c>
     </row>
-    <row r="110" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -16066,8 +16807,11 @@
       <c r="Q110" s="4">
         <v>38.5</v>
       </c>
+      <c r="R110" s="9" t="s">
+        <v>1149</v>
+      </c>
     </row>
-    <row r="111" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -16117,8 +16861,11 @@
       <c r="Q111" s="4">
         <v>38</v>
       </c>
+      <c r="R111" s="9" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="112" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -16170,8 +16917,11 @@
       <c r="Q112" s="4">
         <v>36</v>
       </c>
+      <c r="R112" s="9" t="s">
+        <v>1151</v>
+      </c>
     </row>
-    <row r="113" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -16221,8 +16971,11 @@
       <c r="Q113" s="4">
         <v>35.5</v>
       </c>
+      <c r="R113" s="9" t="s">
+        <v>1149</v>
+      </c>
     </row>
-    <row r="114" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -16272,8 +17025,11 @@
       <c r="Q114" s="4">
         <v>34.5</v>
       </c>
+      <c r="R114" s="9" t="s">
+        <v>1152</v>
+      </c>
     </row>
-    <row r="115" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -16325,8 +17081,11 @@
       <c r="Q115" s="4">
         <v>48</v>
       </c>
+      <c r="R115" s="9" t="s">
+        <v>1122</v>
+      </c>
     </row>
-    <row r="116" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -16378,8 +17137,11 @@
       <c r="Q116" s="4">
         <v>47</v>
       </c>
+      <c r="R116" s="9" t="s">
+        <v>1149</v>
+      </c>
     </row>
-    <row r="117" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -16431,8 +17193,11 @@
       <c r="Q117" s="4">
         <v>46</v>
       </c>
+      <c r="R117" s="9" t="s">
+        <v>1153</v>
+      </c>
     </row>
-    <row r="118" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -16484,8 +17249,11 @@
       <c r="Q118" s="4">
         <v>45</v>
       </c>
+      <c r="R118" s="9" t="s">
+        <v>1154</v>
+      </c>
     </row>
-    <row r="119" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -16537,8 +17305,11 @@
       <c r="Q119" s="4">
         <v>44.5</v>
       </c>
+      <c r="R119" s="9" t="s">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="120" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4"/>
       <c r="B120" s="3" t="s">
         <v>15</v>
@@ -16588,8 +17359,11 @@
       <c r="Q120" s="4">
         <v>44.5</v>
       </c>
+      <c r="R120" s="9" t="s">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="121" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -16641,8 +17415,11 @@
       <c r="Q121" s="4">
         <v>43.5</v>
       </c>
+      <c r="R121" s="9" t="s">
+        <v>1157</v>
+      </c>
     </row>
-    <row r="122" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -16694,8 +17471,11 @@
       <c r="Q122" s="4">
         <v>43</v>
       </c>
+      <c r="R122" s="9" t="s">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="123" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4"/>
       <c r="B123" s="3" t="s">
         <v>15</v>
@@ -16745,8 +17525,11 @@
       <c r="Q123" s="4">
         <v>43</v>
       </c>
+      <c r="R123" s="9" t="s">
+        <v>1159</v>
+      </c>
     </row>
-    <row r="124" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4"/>
       <c r="B124" s="3" t="s">
         <v>15</v>
@@ -16794,8 +17577,11 @@
       <c r="Q124" s="4">
         <v>43</v>
       </c>
+      <c r="R124" s="9" t="s">
+        <v>1119</v>
+      </c>
     </row>
-    <row r="125" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -16847,8 +17633,11 @@
       <c r="Q125" s="4">
         <v>42.5</v>
       </c>
+      <c r="R125" s="9" t="s">
+        <v>1160</v>
+      </c>
     </row>
-    <row r="126" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4"/>
       <c r="B126" s="3" t="s">
         <v>15</v>
@@ -16898,8 +17687,11 @@
       <c r="Q126" s="4">
         <v>42.5</v>
       </c>
+      <c r="R126" s="9" t="s">
+        <v>1161</v>
+      </c>
     </row>
-    <row r="127" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4"/>
       <c r="B127" s="3" t="s">
         <v>15</v>
@@ -16947,8 +17739,11 @@
       <c r="Q127" s="4">
         <v>42.5</v>
       </c>
+      <c r="R127" s="9" t="s">
+        <v>1162</v>
+      </c>
     </row>
-    <row r="128" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4"/>
       <c r="B128" s="3" t="s">
         <v>15</v>
@@ -16996,8 +17791,11 @@
       <c r="Q128" s="4">
         <v>42.5</v>
       </c>
+      <c r="R128" s="9" t="s">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="129" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -17047,8 +17845,11 @@
       <c r="Q129" s="4">
         <v>42</v>
       </c>
+      <c r="R129" s="9" t="s">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="130" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4"/>
       <c r="B130" s="3" t="s">
         <v>15</v>
@@ -17098,8 +17899,11 @@
       <c r="Q130" s="4">
         <v>42</v>
       </c>
+      <c r="R130" s="9" t="s">
+        <v>1164</v>
+      </c>
     </row>
-    <row r="131" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -17149,8 +17953,11 @@
       <c r="Q131" s="4">
         <v>41.5</v>
       </c>
+      <c r="R131" s="9" t="s">
+        <v>1165</v>
+      </c>
     </row>
-    <row r="132" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4"/>
       <c r="B132" s="3" t="s">
         <v>15</v>
@@ -17198,8 +18005,11 @@
       <c r="Q132" s="4">
         <v>41.5</v>
       </c>
+      <c r="R132" s="9" t="s">
+        <v>1166</v>
+      </c>
     </row>
-    <row r="133" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4"/>
       <c r="B133" s="3" t="s">
         <v>15</v>
@@ -17247,8 +18057,11 @@
       <c r="Q133" s="4">
         <v>41.5</v>
       </c>
+      <c r="R133" s="9" t="s">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="134" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4"/>
       <c r="B134" s="3" t="s">
         <v>15</v>
@@ -17298,8 +18111,11 @@
       <c r="Q134" s="4">
         <v>41.5</v>
       </c>
+      <c r="R134" s="9" t="s">
+        <v>1167</v>
+      </c>
     </row>
-    <row r="135" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -17351,8 +18167,11 @@
       <c r="Q135" s="4">
         <v>40.5</v>
       </c>
+      <c r="R135" s="9" t="s">
+        <v>1168</v>
+      </c>
     </row>
-    <row r="136" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -17404,8 +18223,11 @@
       <c r="Q136" s="4">
         <v>40</v>
       </c>
+      <c r="R136" s="9" t="s">
+        <v>1161</v>
+      </c>
     </row>
-    <row r="137" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4"/>
       <c r="B137" s="3" t="s">
         <v>15</v>
@@ -17455,8 +18277,11 @@
       <c r="Q137" s="4">
         <v>40</v>
       </c>
+      <c r="R137" s="9" t="s">
+        <v>1169</v>
+      </c>
     </row>
-    <row r="138" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4"/>
       <c r="B138" s="3" t="s">
         <v>15</v>
@@ -17506,8 +18331,11 @@
       <c r="Q138" s="4">
         <v>40</v>
       </c>
+      <c r="R138" s="9" t="s">
+        <v>1170</v>
+      </c>
     </row>
-    <row r="139" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4"/>
       <c r="B139" s="3" t="s">
         <v>15</v>
@@ -17555,8 +18383,11 @@
       <c r="Q139" s="4">
         <v>40</v>
       </c>
+      <c r="R139" s="9" t="s">
+        <v>1171</v>
+      </c>
     </row>
-    <row r="140" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -17606,8 +18437,11 @@
       <c r="Q140" s="4">
         <v>39.5</v>
       </c>
+      <c r="R140" s="9" t="s">
+        <v>1172</v>
+      </c>
     </row>
-    <row r="141" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -17659,8 +18493,11 @@
       <c r="Q141" s="4">
         <v>39</v>
       </c>
+      <c r="R141" s="9" t="s">
+        <v>1173</v>
+      </c>
     </row>
-    <row r="142" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4"/>
       <c r="B142" s="3" t="s">
         <v>15</v>
@@ -17708,8 +18545,11 @@
       <c r="Q142" s="4">
         <v>39</v>
       </c>
+      <c r="R142" s="9" t="s">
+        <v>1174</v>
+      </c>
     </row>
-    <row r="143" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -17761,8 +18601,11 @@
       <c r="Q143" s="4">
         <v>38</v>
       </c>
+      <c r="R143" s="9" t="s">
+        <v>1175</v>
+      </c>
     </row>
-    <row r="144" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -17812,8 +18655,11 @@
       <c r="Q144" s="4">
         <v>37</v>
       </c>
+      <c r="R144" s="9" t="s">
+        <v>1176</v>
+      </c>
     </row>
-    <row r="145" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -17865,8 +18711,11 @@
       <c r="Q145" s="4">
         <v>36.5</v>
       </c>
+      <c r="R145" s="9" t="s">
+        <v>1177</v>
+      </c>
     </row>
-    <row r="146" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -17918,8 +18767,11 @@
       <c r="Q146" s="4">
         <v>36</v>
       </c>
+      <c r="R146" s="9" t="s">
+        <v>1178</v>
+      </c>
     </row>
-    <row r="147" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -17971,8 +18823,11 @@
       <c r="Q147" s="4">
         <v>35.5</v>
       </c>
+      <c r="R147" s="9" t="s">
+        <v>1145</v>
+      </c>
     </row>
-    <row r="148" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4"/>
       <c r="B148" s="3" t="s">
         <v>15</v>
@@ -18022,8 +18877,11 @@
       <c r="Q148" s="4">
         <v>35.5</v>
       </c>
+      <c r="R148" s="9" t="s">
+        <v>1179</v>
+      </c>
     </row>
-    <row r="149" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -18073,8 +18931,11 @@
       <c r="Q149" s="4">
         <v>35</v>
       </c>
+      <c r="R149" s="9" t="s">
+        <v>1180</v>
+      </c>
     </row>
-    <row r="150" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -18124,8 +18985,11 @@
       <c r="Q150" s="4">
         <v>33.5</v>
       </c>
+      <c r="R150" s="9" t="s">
+        <v>1181</v>
+      </c>
     </row>
-    <row r="151" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -18175,11 +19039,14 @@
       <c r="Q151" s="4">
         <v>32.5</v>
       </c>
+      <c r="R151" s="9" t="s">
+        <v>1182</v>
+      </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" s="1"/>
     </row>
   </sheetData>

</xml_diff>